<commit_message>
Funished schematics and GPIO drv interface
</commit_message>
<xml_diff>
--- a/Resources/Calculations.xlsx
+++ b/Resources/Calculations.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ElektronicznyDeVeLoPiNg\Weatherever\Weather-ever\Resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ElektronicznyDeVeLoPiNg\Weatherever\Weatherever\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4A22F30-B97D-4BDD-B971-F59F5C675631}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A4D026C-B6F6-4D9A-BD50-10CB048C7029}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5715" yWindow="1590" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>R1</t>
   </si>
@@ -85,6 +85,9 @@
   </si>
   <si>
     <t>Y102</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  </t>
   </si>
 </sst>
 </file>
@@ -515,8 +518,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -546,15 +549,15 @@
         <v>0</v>
       </c>
       <c r="B3">
-        <v>80000</v>
+        <v>47000</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>1</v>
       </c>
-      <c r="B4">
-        <v>80000</v>
+      <c r="B4" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -579,9 +582,9 @@
       <c r="A7" t="s">
         <v>6</v>
       </c>
-      <c r="B7">
+      <c r="B7" t="e">
         <f>B2*(B3/(B3+B4))</f>
-        <v>4.5</v>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -604,18 +607,18 @@
       <c r="A10" t="s">
         <v>4</v>
       </c>
-      <c r="B10">
+      <c r="B10" t="e">
         <f>((B5+B6)*B7-(B5*B9))/B6</f>
-        <v>5.45</v>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>5</v>
       </c>
-      <c r="B11">
+      <c r="B11" t="e">
         <f>((B5+B6)*B7-(B5*B8))/B6</f>
-        <v>3.375</v>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>